<commit_message>
Actualización de mi forma-logt1.
</commit_message>
<xml_diff>
--- a/tspi/ciclo-1/forma-logt1-20106065.xlsx
+++ b/tspi/ciclo-1/forma-logt1-20106065.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Terminé la creación del esquema del documento de requerimientos.</t>
+  </si>
+  <si>
+    <t>Reunión de Equipo</t>
+  </si>
+  <si>
+    <t>Tuvimos una reunión de equipo para la asignación de las tareas del ciclo #1.</t>
   </si>
 </sst>
 </file>
@@ -198,11 +204,14 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
@@ -253,92 +262,95 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E14" activeCellId="0" pane="topLeft" sqref="E14"/>
+      <selection activeCell="F9" activeCellId="0" pane="topLeft" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="16.4588235294118"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.8156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.3960784313726"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="46.5254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="4" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="16.5411764705882"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.8705882352941"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="16.8862745098039"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="46.7607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="E1" s="8" t="s">
+      <c r="C1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9" t="n">
+      <c r="F1" s="10" t="n">
         <v>41905</v>
       </c>
-      <c r="G1" s="9"/>
+      <c r="G1" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="11"/>
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="11"/>
+      <c r="G2" s="12"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="E3" s="8" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="E3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="11" t="n">
+      <c r="F3" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="11"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="4">
+      <c r="F4" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="5">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -362,7 +374,7 @@
       <c r="F6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -386,7 +398,7 @@
       <c r="F7" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -410,7 +422,7 @@
       <c r="F8" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -434,7 +446,7 @@
       <c r="F9" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -458,7 +470,7 @@
       <c r="F10" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -482,7 +494,7 @@
       <c r="F11" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -506,8 +518,32 @@
       <c r="F12" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="6" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="13">
+      <c r="A13" s="1" t="n">
+        <v>41912</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>0.96875</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>0.993055555555556</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <f aca="false">((HOUR(C13)-HOUR(B13))*60)+(MINUTE(C13)-MINUTE(B13))-D13</f>
+        <v>35</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>